<commit_message>
Fixed an error in a spelling
Former-commit-id: dfa659d620d9f91e680b07daf44390a71605b9ff
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Leagues.xlsx
+++ b/Docs/Content/HungryDragonContent_Leagues.xlsx
@@ -392,7 +392,7 @@
     <t>egg_offer</t>
   </si>
   <si>
-    <t>egg_betterRate</t>
+    <t>egg_betterRates</t>
   </si>
 </sst>
 </file>
@@ -1268,8 +1268,8 @@
   </sheetPr>
   <dimension ref="A1:J72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1280,7 +1280,7 @@
     <col min="4" max="4" width="10" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" customWidth="1"/>
     <col min="6" max="6" width="11.85546875" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" customWidth="1"/>
     <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20.42578125" customWidth="1"/>

</xml_diff>